<commit_message>
TeensyEWMU: update pinout sheet to call out crossover style IDC26-to-DB25 cable usage
</commit_message>
<xml_diff>
--- a/src/SimLinkup/HardwareSupport/TeensyEWMU/PCB/CMDS_EWMU_EWPI Driver Board rev 1_01 - D-Sub Connector Pinouts 2021-05-24.xlsx
+++ b/src/SimLinkup/HardwareSupport/TeensyEWMU/PCB/CMDS_EWMU_EWPI Driver Board rev 1_01 - D-Sub Connector Pinouts 2021-05-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lightningstools\src\SimLinkup\HardwareSupport\TeensyEWMU\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CFAE35-8F2A-416B-9C81-C190D88F6AC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B94442-0665-43D8-ABD9-C4924238CD7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{922FAF36-AAD4-4B14-8DEE-245AF8D4A57E}"/>
   </bookViews>
@@ -385,23 +385,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">EWMU / CMDS
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CN1 (IDC 2X13 PIN HEADER)
-TO DB-25 MALE (STRAIGHT THRU)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">EWPI
 </t>
     </r>
@@ -441,6 +424,23 @@
   </si>
   <si>
     <t>IDC 10 PIN</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">EWMU / CMDS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CN1 (IDC 2X13 PIN HEADER)
+TO DB-25 MALE (PARALLEL PORT TYPE)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -970,6 +970,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1006,6 +1018,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1017,21 +1032,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1349,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238C02CC-6C06-454B-89D2-F571954FD99C}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.35"/>
@@ -1375,73 +1375,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="71"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="75"/>
       <c r="H1" s="28"/>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="66"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="70"/>
     </row>
     <row r="2" spans="1:17" ht="10.9" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="72"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="78"/>
       <c r="H2" s="29"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="69"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="73"/>
     </row>
     <row r="3" spans="1:17" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="75"/>
       <c r="D3" s="15"/>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="70"/>
-      <c r="G3" s="71"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="75"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="77" t="s">
+      <c r="I3" s="82" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="71"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="75"/>
     </row>
     <row r="4" spans="1:17" s="60" customFormat="1" ht="34.9" x14ac:dyDescent="0.45">
       <c r="A4" s="53" t="s">
@@ -1468,10 +1468,10 @@
         <v>89</v>
       </c>
       <c r="J4" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="K4" s="83" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="K4" s="66" t="s">
+        <v>110</v>
       </c>
       <c r="L4" s="59" t="s">
         <v>90</v>
@@ -1481,10 +1481,10 @@
         <v>89</v>
       </c>
       <c r="O4" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="P4" s="80" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="P4" s="64" t="s">
+        <v>111</v>
       </c>
       <c r="Q4" s="55" t="s">
         <v>90</v>
@@ -1517,7 +1517,7 @@
       <c r="J5" s="16">
         <v>1</v>
       </c>
-      <c r="K5" s="84">
+      <c r="K5" s="67">
         <v>1</v>
       </c>
       <c r="L5" s="20" t="s">
@@ -1530,7 +1530,7 @@
       <c r="O5" s="17">
         <v>1</v>
       </c>
-      <c r="P5" s="81">
+      <c r="P5" s="65">
         <v>1</v>
       </c>
       <c r="Q5" s="19" t="s">
@@ -1567,7 +1567,7 @@
         <f>J5+1</f>
         <v>2</v>
       </c>
-      <c r="K6" s="84">
+      <c r="K6" s="67">
         <v>14</v>
       </c>
       <c r="L6" s="30" t="s">
@@ -1581,7 +1581,7 @@
         <f>O5+1</f>
         <v>2</v>
       </c>
-      <c r="P6" s="81">
+      <c r="P6" s="65">
         <v>2</v>
       </c>
       <c r="Q6" s="20" t="s">
@@ -1618,7 +1618,7 @@
         <f t="shared" ref="J7" si="2">J6+1</f>
         <v>3</v>
       </c>
-      <c r="K7" s="84">
+      <c r="K7" s="67">
         <v>2</v>
       </c>
       <c r="L7" s="20" t="s">
@@ -1632,7 +1632,7 @@
         <f t="shared" ref="O7:O13" si="3">O6+1</f>
         <v>3</v>
       </c>
-      <c r="P7" s="81">
+      <c r="P7" s="65">
         <v>3</v>
       </c>
       <c r="Q7" s="20" t="s">
@@ -1669,7 +1669,7 @@
         <f t="shared" ref="J8" si="4">J7+1</f>
         <v>4</v>
       </c>
-      <c r="K8" s="84">
+      <c r="K8" s="67">
         <v>15</v>
       </c>
       <c r="L8" s="20" t="s">
@@ -1683,7 +1683,7 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="P8" s="81">
+      <c r="P8" s="65">
         <v>4</v>
       </c>
       <c r="Q8" s="23" t="s">
@@ -1720,7 +1720,7 @@
         <f t="shared" ref="J9" si="5">J8+1</f>
         <v>5</v>
       </c>
-      <c r="K9" s="84">
+      <c r="K9" s="67">
         <v>3</v>
       </c>
       <c r="L9" s="20" t="s">
@@ -1734,7 +1734,7 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="P9" s="81">
+      <c r="P9" s="65">
         <v>5</v>
       </c>
       <c r="Q9" s="19" t="s">
@@ -1771,7 +1771,7 @@
         <f t="shared" ref="J10" si="6">J9+1</f>
         <v>6</v>
       </c>
-      <c r="K10" s="84">
+      <c r="K10" s="67">
         <v>16</v>
       </c>
       <c r="L10" s="20" t="s">
@@ -1785,7 +1785,7 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="P10" s="81">
+      <c r="P10" s="65">
         <v>6</v>
       </c>
       <c r="Q10" s="19" t="s">
@@ -1822,7 +1822,7 @@
         <f t="shared" ref="J11" si="7">J10+1</f>
         <v>7</v>
       </c>
-      <c r="K11" s="84">
+      <c r="K11" s="67">
         <v>4</v>
       </c>
       <c r="L11" s="20" t="s">
@@ -1836,7 +1836,7 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="P11" s="81">
+      <c r="P11" s="65">
         <v>7</v>
       </c>
       <c r="Q11" s="19" t="s">
@@ -1873,7 +1873,7 @@
         <f t="shared" ref="J12" si="8">J11+1</f>
         <v>8</v>
       </c>
-      <c r="K12" s="84">
+      <c r="K12" s="67">
         <v>17</v>
       </c>
       <c r="L12" s="20" t="s">
@@ -1887,7 +1887,7 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="P12" s="81">
+      <c r="P12" s="65">
         <v>8</v>
       </c>
       <c r="Q12" s="19" t="s">
@@ -1924,7 +1924,7 @@
         <f t="shared" ref="J13" si="9">J12+1</f>
         <v>9</v>
       </c>
-      <c r="K13" s="84">
+      <c r="K13" s="67">
         <v>5</v>
       </c>
       <c r="L13" s="20" t="s">
@@ -1938,7 +1938,7 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="P13" s="81">
+      <c r="P13" s="65">
         <v>9</v>
       </c>
       <c r="Q13" s="19" t="s">
@@ -1975,7 +1975,7 @@
         <f t="shared" ref="J14" si="10">J13+1</f>
         <v>10</v>
       </c>
-      <c r="K14" s="84">
+      <c r="K14" s="67">
         <v>18</v>
       </c>
       <c r="L14" s="20" t="s">
@@ -1988,7 +1988,7 @@
       <c r="O14" s="17">
         <v>10</v>
       </c>
-      <c r="P14" s="81" t="s">
+      <c r="P14" s="65" t="s">
         <v>9</v>
       </c>
       <c r="Q14" s="19" t="s">
@@ -2025,7 +2025,7 @@
         <f>J14+1</f>
         <v>11</v>
       </c>
-      <c r="K15" s="84">
+      <c r="K15" s="67">
         <v>6</v>
       </c>
       <c r="L15" s="20" t="s">
@@ -2067,7 +2067,7 @@
         <f>J15+1</f>
         <v>12</v>
       </c>
-      <c r="K16" s="84">
+      <c r="K16" s="67">
         <v>19</v>
       </c>
       <c r="L16" s="20" t="s">
@@ -2109,7 +2109,7 @@
         <f t="shared" ref="J17" si="11">J16+1</f>
         <v>13</v>
       </c>
-      <c r="K17" s="84">
+      <c r="K17" s="67">
         <v>7</v>
       </c>
       <c r="L17" s="20" t="s">
@@ -2151,7 +2151,7 @@
         <f t="shared" ref="J18" si="12">J17+1</f>
         <v>14</v>
       </c>
-      <c r="K18" s="84">
+      <c r="K18" s="67">
         <v>20</v>
       </c>
       <c r="L18" s="20" t="s">
@@ -2176,14 +2176,14 @@
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F19" s="17">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="18" t="s">
@@ -2193,7 +2193,7 @@
         <f t="shared" ref="J19" si="13">J18+1</f>
         <v>15</v>
       </c>
-      <c r="K19" s="84">
+      <c r="K19" s="67">
         <v>8</v>
       </c>
       <c r="L19" s="20" t="s">
@@ -2207,14 +2207,14 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="B20" s="17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="22" t="s">
@@ -2235,7 +2235,7 @@
         <f t="shared" ref="J20" si="14">J19+1</f>
         <v>16</v>
       </c>
-      <c r="K20" s="84">
+      <c r="K20" s="67">
         <v>21</v>
       </c>
       <c r="L20" s="20" t="s">
@@ -2249,14 +2249,14 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="17">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="B21" s="17">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="22" t="s">
@@ -2277,7 +2277,7 @@
         <f t="shared" ref="J21" si="15">J20+1</f>
         <v>17</v>
       </c>
-      <c r="K21" s="84">
+      <c r="K21" s="67">
         <v>9</v>
       </c>
       <c r="L21" s="20" t="s">
@@ -2319,7 +2319,7 @@
         <f t="shared" ref="J22" si="16">J21+1</f>
         <v>18</v>
       </c>
-      <c r="K22" s="84">
+      <c r="K22" s="67">
         <v>22</v>
       </c>
       <c r="L22" s="20" t="s">
@@ -2361,7 +2361,7 @@
         <f t="shared" ref="J23" si="17">J22+1</f>
         <v>19</v>
       </c>
-      <c r="K23" s="84">
+      <c r="K23" s="67">
         <v>10</v>
       </c>
       <c r="L23" s="20" t="s">
@@ -2403,7 +2403,7 @@
         <f t="shared" ref="J24" si="18">J23+1</f>
         <v>20</v>
       </c>
-      <c r="K24" s="84">
+      <c r="K24" s="67">
         <v>23</v>
       </c>
       <c r="L24" s="20" t="s">
@@ -2445,7 +2445,7 @@
         <f t="shared" ref="J25" si="19">J24+1</f>
         <v>21</v>
       </c>
-      <c r="K25" s="84">
+      <c r="K25" s="67">
         <v>11</v>
       </c>
       <c r="L25" s="20" t="s">
@@ -2487,7 +2487,7 @@
         <f t="shared" ref="J26" si="20">J25+1</f>
         <v>22</v>
       </c>
-      <c r="K26" s="84">
+      <c r="K26" s="67">
         <v>24</v>
       </c>
       <c r="L26" s="20" t="s">
@@ -2529,7 +2529,7 @@
         <f t="shared" ref="J27" si="21">J26+1</f>
         <v>23</v>
       </c>
-      <c r="K27" s="84">
+      <c r="K27" s="67">
         <v>12</v>
       </c>
       <c r="L27" s="20" t="s">
@@ -2571,7 +2571,7 @@
         <f t="shared" ref="J28" si="22">J27+1</f>
         <v>24</v>
       </c>
-      <c r="K28" s="84">
+      <c r="K28" s="67">
         <v>25</v>
       </c>
       <c r="L28" s="20" t="s">
@@ -2613,7 +2613,7 @@
         <f t="shared" ref="J29" si="23">J28+1</f>
         <v>25</v>
       </c>
-      <c r="K29" s="84">
+      <c r="K29" s="67">
         <v>13</v>
       </c>
       <c r="L29" s="20" t="s">
@@ -2647,7 +2647,7 @@
       <c r="J30" s="16">
         <v>26</v>
       </c>
-      <c r="K30" s="84" t="s">
+      <c r="K30" s="67" t="s">
         <v>9</v>
       </c>
       <c r="L30" s="20" t="s">
@@ -2889,11 +2889,11 @@
       <c r="L39" s="61"/>
       <c r="M39" s="44"/>
       <c r="N39" s="43"/>
-      <c r="O39" s="75" t="s">
-        <v>109</v>
-      </c>
-      <c r="P39" s="82"/>
-      <c r="Q39" s="76"/>
+      <c r="O39" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="P39" s="80"/>
+      <c r="Q39" s="81"/>
     </row>
     <row r="40" spans="1:17" ht="14.65" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="22" t="s">
@@ -2945,7 +2945,7 @@
       <c r="J41" s="42"/>
       <c r="K41" s="42"/>
       <c r="L41" s="63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M41" s="49"/>
       <c r="N41" s="50" t="s">

</xml_diff>